<commit_message>
fix(import) : memperbaiki import di gambar
</commit_message>
<xml_diff>
--- a/public/template_barang.xlsx
+++ b/public/template_barang.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\File untuk kuliah\semester-4\Pemrograman Web Lanjut\P8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\pwl_pos\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61725DED-6F08-4605-9445-35BCCCD7D616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D35AFFA6-4534-462C-9FF8-048B51A1E635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB775108-128B-4670-B73F-432BC8A16FBB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EA3E68DD-1269-4BB3-99BD-2D01BC9843CE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Lembar1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>kategori_id</t>
   </si>
@@ -42,52 +53,31 @@
     <t>harga_jual</t>
   </si>
   <si>
-    <t>BRG001</t>
-  </si>
-  <si>
-    <t>BRG002</t>
-  </si>
-  <si>
-    <t>BRG003</t>
-  </si>
-  <si>
-    <t>BRG004</t>
-  </si>
-  <si>
-    <t>BRG005</t>
-  </si>
-  <si>
-    <t>Esteh</t>
-  </si>
-  <si>
-    <t>Es Jeruk</t>
-  </si>
-  <si>
-    <t>Soda Gembira</t>
-  </si>
-  <si>
-    <t>Nasi Goreng</t>
-  </si>
-  <si>
-    <t>Ayam Goreng</t>
-  </si>
-  <si>
-    <t>BRG006</t>
-  </si>
-  <si>
-    <t>Steak</t>
-  </si>
-  <si>
-    <t>BRG007</t>
-  </si>
-  <si>
-    <t>Panci</t>
-  </si>
-  <si>
-    <t>BRG008</t>
-  </si>
-  <si>
-    <t>Wajan</t>
+    <t>SBK-003</t>
+  </si>
+  <si>
+    <t>SNK-003</t>
+  </si>
+  <si>
+    <t>MND-003</t>
+  </si>
+  <si>
+    <t>BAY-003</t>
+  </si>
+  <si>
+    <t>MNM-003</t>
+  </si>
+  <si>
+    <t>Telur Omega</t>
+  </si>
+  <si>
+    <t>Sari Roti</t>
+  </si>
+  <si>
+    <t>Shampo Pantene</t>
+  </si>
+  <si>
+    <t>Cleo 600ml</t>
   </si>
   <si>
     <t>Baju epep</t>
@@ -101,25 +91,22 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
-      <charset val="1"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-      <scheme val="minor"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -142,9 +129,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -163,9 +151,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -173,39 +161,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -257,7 +245,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -309,7 +297,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -368,13 +356,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -383,6 +364,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -447,25 +435,52 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25C4D8A8-6452-4100-9DE1-AB5FC7D5D222}">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFAAAB3A-9AD9-4191-A7B4-04B63F9C1C81}">
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -485,160 +500,92 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2">
-        <v>10000</v>
-      </c>
-      <c r="E2">
-        <v>35000</v>
+      <c r="D2" s="2">
+        <v>22000</v>
+      </c>
+      <c r="E2" s="2">
+        <v>25000</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3">
-        <v>15000</v>
-      </c>
-      <c r="E3">
-        <v>25000</v>
+      <c r="D3" s="2">
+        <v>11500</v>
+      </c>
+      <c r="E3" s="2">
+        <v>12500</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4">
-        <v>20000</v>
-      </c>
-      <c r="E4">
-        <v>35000</v>
+      <c r="D4" s="2">
+        <v>17500</v>
+      </c>
+      <c r="E4" s="2">
+        <v>18500</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5">
-        <v>30000</v>
-      </c>
-      <c r="E5">
-        <v>45000</v>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2">
+        <v>89000</v>
+      </c>
+      <c r="E5" s="2">
+        <v>92500</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6">
-        <v>40000</v>
-      </c>
-      <c r="E6">
-        <v>55000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7">
-        <v>50000</v>
-      </c>
-      <c r="E7">
-        <v>65000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8">
-        <v>60000</v>
-      </c>
-      <c r="E8">
-        <v>75000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9">
-        <v>70000</v>
-      </c>
-      <c r="E9">
-        <v>85000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>4</v>
-      </c>
-      <c r="B10">
-        <v>1234</v>
-      </c>
-      <c r="C10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10">
-        <v>2000</v>
-      </c>
-      <c r="E10">
-        <v>3000</v>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3750</v>
+      </c>
+      <c r="E6" s="2">
+        <v>4300</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>